<commit_message>
Added Project output to R Code, generated output
</commit_message>
<xml_diff>
--- a/Data/Habitat_Limiting_Factor_Rating_Criteria.xlsx
+++ b/Data/Habitat_Limiting_Factor_Rating_Criteria.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\Documents\GitHub\Prioritization_Step2_Data_R_Project\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27E53FD1-DA4A-4719-890E-2B4723E4FBDD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0FFE386-F5E4-4888-9E2A-55618D9F99AF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="912" windowWidth="15900" windowHeight="11448" xr2:uid="{39DD5E77-4161-45F8-A228-94BEA2686D53}"/>
+    <workbookView xWindow="5244" yWindow="3084" windowWidth="17280" windowHeight="10560" xr2:uid="{39DD5E77-4161-45F8-A228-94BEA2686D53}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3753,16 +3753,16 @@
   <dimension ref="A1:O100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="O49" sqref="O49"/>
+      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="48.77734375" customWidth="1"/>
     <col min="2" max="3" width="26.44140625" customWidth="1"/>
-    <col min="4" max="4" width="94.5546875" customWidth="1"/>
+    <col min="4" max="4" width="65" customWidth="1"/>
     <col min="5" max="8" width="26.44140625" customWidth="1"/>
     <col min="9" max="11" width="13" customWidth="1"/>
     <col min="12" max="12" width="8.88671875" style="35"/>

</xml_diff>